<commit_message>
updated standard 1163 excel file
</commit_message>
<xml_diff>
--- a/HeraGPT/src/NzStandards/Excel/AS-NZS 1163.xlsx
+++ b/HeraGPT/src/NzStandards/Excel/AS-NZS 1163.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/GitHub/AI_MATERIAL_COMPLIANCE/HeraGPT/src/NzStandards/Excel/1163 - 2016/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xkrym\Desktop\Git\AI_MATERIAL_COMPLIANCE\HeraGPT\src\NzStandards\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3A5AF3-EA90-6B4F-B50B-A0D281E11C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C18996-1FE6-4162-AAC9-5F9C5FB19E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="1640" windowWidth="20100" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>&lt;=</t>
   </si>
@@ -95,38 +95,44 @@
     <t>C450,C450L2</t>
   </si>
   <si>
-    <t>Circular&lt;=15</t>
-  </si>
-  <si>
-    <t>&gt;15</t>
-  </si>
-  <si>
-    <t>&lt;=30</t>
-  </si>
-  <si>
     <t>&gt;30</t>
   </si>
   <si>
-    <t>minimum_yield_strength</t>
-  </si>
-  <si>
-    <t>minimum_tensile_strength</t>
-  </si>
-  <si>
-    <t>rectangular&lt;=15</t>
-  </si>
-  <si>
     <t>TENSILE TEST REQUIREMENTS</t>
   </si>
   <si>
     <t>CHEMICAL COMPOSITIONS</t>
+  </si>
+  <si>
+    <t>&gt;15 ≤30</t>
+  </si>
+  <si>
+    <t>C350,C350L0</t>
+  </si>
+  <si>
+    <t>C450,C450L0</t>
+  </si>
+  <si>
+    <t>Circular hollow sections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">≤15 </t>
+  </si>
+  <si>
+    <t>Minimum yield strength</t>
+  </si>
+  <si>
+    <t>Minimum tensile strength</t>
+  </si>
+  <si>
+    <t>Rectangular hollow sections</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,13 +148,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -163,10 +181,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,131 +501,246 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:R20"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.83203125" customWidth="1"/>
-    <col min="11" max="11" width="24.83203125" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" customWidth="1"/>
     <col min="17" max="17" width="27" customWidth="1"/>
-    <col min="18" max="18" width="25.33203125" customWidth="1"/>
+    <col min="18" max="18" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" t="s">
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
-        <v>0</v>
-      </c>
-      <c r="L4" t="s">
-        <v>0</v>
-      </c>
-      <c r="N4" t="s">
-        <v>0</v>
-      </c>
-      <c r="O4" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>0</v>
-      </c>
-      <c r="R4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N5" t="s">
+      <c r="M3" s="2"/>
+      <c r="N3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="L4">
+        <v>0.25</v>
+      </c>
+      <c r="N4">
+        <v>0.25</v>
+      </c>
+      <c r="O4">
+        <v>0.25</v>
+      </c>
+      <c r="Q4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="L5">
+        <v>0.43</v>
+      </c>
+      <c r="N5">
+        <v>0.25</v>
+      </c>
+      <c r="O5">
+        <v>0.25</v>
+      </c>
+      <c r="R5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="C6" s="1">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="D6" s="1">
-        <v>0.5</v>
+        <v>1.7</v>
       </c>
       <c r="E6" s="1">
         <v>0.03</v>
@@ -614,10 +749,10 @@
         <v>0.03</v>
       </c>
       <c r="G6" s="1">
-        <v>0.15</v>
+        <v>0.03</v>
       </c>
       <c r="H6" s="1">
-        <v>0.1</v>
+        <v>0.35</v>
       </c>
       <c r="I6" s="1">
         <v>0.1</v>
@@ -626,10 +761,10 @@
         <v>0.04</v>
       </c>
       <c r="K6" s="1">
-        <v>0.03</v>
+        <v>0.15</v>
       </c>
       <c r="L6">
-        <v>0.25</v>
+        <v>0.43</v>
       </c>
       <c r="N6">
         <v>0.25</v>
@@ -637,262 +772,177 @@
       <c r="O6">
         <v>0.25</v>
       </c>
-      <c r="Q6">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="H7" s="1">
+      <c r="R6">
         <v>0.1</v>
       </c>
-      <c r="I7" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="K7" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="L7">
-        <v>0.43</v>
-      </c>
-      <c r="N7">
-        <v>0.25</v>
-      </c>
-      <c r="O7">
-        <v>0.25</v>
-      </c>
-      <c r="R7">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1.7</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0.35</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="K8" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="L8">
-        <v>0.43</v>
-      </c>
-      <c r="N8">
-        <v>0.25</v>
-      </c>
-      <c r="O8">
-        <v>0.25</v>
-      </c>
-      <c r="R8">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
       </c>
       <c r="E12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13">
+        <v>250</v>
+      </c>
+      <c r="C13">
+        <v>320</v>
+      </c>
+      <c r="D13">
         <v>18</v>
       </c>
-      <c r="C13">
+      <c r="E13">
         <v>20</v>
       </c>
-      <c r="D13">
+      <c r="F13">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>350</v>
+      </c>
+      <c r="C14">
+        <v>430</v>
+      </c>
+      <c r="D14">
+        <v>16</v>
+      </c>
+      <c r="E14">
+        <v>28</v>
+      </c>
+      <c r="F14">
         <v>20</v>
       </c>
-      <c r="E13">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14">
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>450</v>
+      </c>
+      <c r="C15">
+        <v>500</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
+      </c>
+      <c r="E15">
+        <v>14</v>
+      </c>
+      <c r="F15">
         <v>16</v>
       </c>
-      <c r="C14">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
         <v>28</v>
       </c>
-      <c r="D14">
-        <v>28</v>
-      </c>
-      <c r="E14">
-        <v>20</v>
-      </c>
-      <c r="G14" t="s">
-        <v>23</v>
-      </c>
-      <c r="H14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15">
-        <v>12</v>
-      </c>
-      <c r="C15">
-        <v>24</v>
-      </c>
-      <c r="D15">
-        <v>24</v>
-      </c>
-      <c r="E15">
-        <v>16</v>
-      </c>
-      <c r="G15">
-        <v>250</v>
-      </c>
-      <c r="H15">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="G16">
-        <v>350</v>
-      </c>
-      <c r="H16">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E17" t="s">
         <v>22</v>
       </c>
-      <c r="G17">
-        <v>450</v>
-      </c>
-      <c r="H17">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18">
+        <v>250</v>
+      </c>
+      <c r="C18">
+        <v>320</v>
+      </c>
+      <c r="D18">
         <v>14</v>
       </c>
-      <c r="C18">
+      <c r="E18">
         <v>16</v>
       </c>
-      <c r="D18">
-        <v>16</v>
-      </c>
-      <c r="E18">
+      <c r="F18">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19">
+        <v>350</v>
+      </c>
+      <c r="C19">
+        <v>430</v>
+      </c>
+      <c r="D19">
         <v>12</v>
       </c>
-      <c r="C19">
+      <c r="E19">
         <v>14</v>
       </c>
-      <c r="D19">
-        <v>14</v>
-      </c>
-      <c r="E19">
+      <c r="F19">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20">
+        <v>450</v>
+      </c>
+      <c r="C20">
+        <v>500</v>
+      </c>
+      <c r="D20">
         <v>10</v>
       </c>
-      <c r="C20">
+      <c r="E20">
         <v>12</v>
       </c>
-      <c r="D20">
-        <v>12</v>
-      </c>
-      <c r="E20">
+      <c r="F20">
         <v>14</v>
       </c>
     </row>
@@ -913,15 +963,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100492A33985A8189488130B17E2737950F" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0600126c02bf7d96f3f71331012d5124">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fcad6362-6db2-4142-813e-fbcb646a0851" xmlns:ns3="8570f440-dc23-4bae-a484-35cf4850d8e4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1bd227723330db67820ac8dc89a16092" ns2:_="" ns3:_="">
     <xsd:import namespace="fcad6362-6db2-4142-813e-fbcb646a0851"/>
@@ -1122,6 +1163,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B446E7F-3CD5-4867-AB34-0922B1F29BF8}">
   <ds:schemaRefs>
@@ -1134,14 +1184,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F95EEE24-BE14-48A0-990C-53670D7C83A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C01599A-DE44-4319-8DB0-ED4CA7CF8A71}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1158,4 +1200,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F95EEE24-BE14-48A0-990C-53670D7C83A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>